<commit_message>
Update K3 DS & RM
</commit_message>
<xml_diff>
--- a/S32K3/S32K3xx_DMAMUX_map.xlsx
+++ b/S32K3/S32K3xx_DMAMUX_map.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\ccwork\AUTO\012_systems_table_generator\SW\python\table_generation\out\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF48AA4-DB53-4958-984E-D389B9FD1111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1522" yWindow="1522" windowWidth="36027" windowHeight="16831" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DMAMUX0" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DMAMUX0!$D$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DMAMUX1!$D$1:$Q$1</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -420,8 +426,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +513,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -553,7 +567,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -585,9 +599,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -619,6 +651,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -794,39 +844,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="2" max="2" width="9.75" customWidth="1"/>
+    <col min="3" max="3" width="27.75" customWidth="1"/>
+    <col min="4" max="18" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="12" customHeight="1">
+    <row r="1" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -876,7 +912,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="12" customHeight="1">
+    <row r="2" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -898,7 +934,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="44.15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -954,7 +990,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="12" customHeight="1">
+    <row r="4" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1008,7 +1044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12" customHeight="1">
+    <row r="5" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1064,7 +1100,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="12" customHeight="1">
+    <row r="6" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1120,7 +1156,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="12" customHeight="1">
+    <row r="7" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1176,7 +1212,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="12" customHeight="1">
+    <row r="8" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1232,7 +1268,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="12" customHeight="1">
+    <row r="9" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1288,7 +1324,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="12" customHeight="1">
+    <row r="10" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1344,7 +1380,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="12" customHeight="1">
+    <row r="11" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1400,7 +1436,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="12" customHeight="1">
+    <row r="12" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1456,7 +1492,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="12" customHeight="1">
+    <row r="13" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -1512,7 +1548,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="12" customHeight="1">
+    <row r="14" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1568,7 +1604,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="12" customHeight="1">
+    <row r="15" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -1624,7 +1660,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="12" customHeight="1">
+    <row r="16" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -1680,7 +1716,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="12" customHeight="1">
+    <row r="17" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1736,7 +1772,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="12" customHeight="1">
+    <row r="18" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1792,7 +1828,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="12" customHeight="1">
+    <row r="19" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1848,7 +1884,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="12" customHeight="1">
+    <row r="20" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1904,7 +1940,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="12" customHeight="1">
+    <row r="21" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1960,7 +1996,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="12" customHeight="1">
+    <row r="22" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -2016,7 +2052,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="12" customHeight="1">
+    <row r="23" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -2072,7 +2108,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="12" customHeight="1">
+    <row r="24" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -2128,7 +2164,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="12" customHeight="1">
+    <row r="25" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -2184,7 +2220,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="12" customHeight="1">
+    <row r="26" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -2240,7 +2276,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="12" customHeight="1">
+    <row r="27" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -2296,7 +2332,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="12" customHeight="1">
+    <row r="28" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -2352,7 +2388,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="12" customHeight="1">
+    <row r="29" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -2408,7 +2444,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="12" customHeight="1">
+    <row r="30" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -2464,7 +2500,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="12" customHeight="1">
+    <row r="31" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -2520,7 +2556,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="12" customHeight="1">
+    <row r="32" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -2574,7 +2610,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="12" customHeight="1">
+    <row r="33" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -2630,7 +2666,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="12" customHeight="1">
+    <row r="34" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -2686,7 +2722,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="12" customHeight="1">
+    <row r="35" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31</v>
       </c>
@@ -2742,7 +2778,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="12" customHeight="1">
+    <row r="36" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>32</v>
       </c>
@@ -2798,7 +2834,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="12" customHeight="1">
+    <row r="37" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>33</v>
       </c>
@@ -2854,7 +2890,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="12" customHeight="1">
+    <row r="38" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>33</v>
       </c>
@@ -2910,7 +2946,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="12" customHeight="1">
+    <row r="39" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>34</v>
       </c>
@@ -2966,7 +3002,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="12" customHeight="1">
+    <row r="40" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>34</v>
       </c>
@@ -3022,7 +3058,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="12" customHeight="1">
+    <row r="41" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>35</v>
       </c>
@@ -3078,7 +3114,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="12" customHeight="1">
+    <row r="42" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>35</v>
       </c>
@@ -3134,7 +3170,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="12" customHeight="1">
+    <row r="43" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>36</v>
       </c>
@@ -3190,7 +3226,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="12" customHeight="1">
+    <row r="44" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>36</v>
       </c>
@@ -3246,7 +3282,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="12" customHeight="1">
+    <row r="45" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>37</v>
       </c>
@@ -3302,7 +3338,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="12" customHeight="1">
+    <row r="46" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>37</v>
       </c>
@@ -3358,7 +3394,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="12" customHeight="1">
+    <row r="47" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>38</v>
       </c>
@@ -3414,7 +3450,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="12" customHeight="1">
+    <row r="48" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>38</v>
       </c>
@@ -3470,7 +3506,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="12" customHeight="1">
+    <row r="49" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>39</v>
       </c>
@@ -3526,7 +3562,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="12" customHeight="1">
+    <row r="50" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>39</v>
       </c>
@@ -3582,7 +3618,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="12" customHeight="1">
+    <row r="51" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>40</v>
       </c>
@@ -3638,7 +3674,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="12" customHeight="1">
+    <row r="52" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>40</v>
       </c>
@@ -3694,7 +3730,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="12" customHeight="1">
+    <row r="53" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>41</v>
       </c>
@@ -3750,7 +3786,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="12" customHeight="1">
+    <row r="54" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>41</v>
       </c>
@@ -3806,7 +3842,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="12" customHeight="1">
+    <row r="55" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>42</v>
       </c>
@@ -3862,7 +3898,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="12" customHeight="1">
+    <row r="56" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>42</v>
       </c>
@@ -3918,7 +3954,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="12" customHeight="1">
+    <row r="57" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43</v>
       </c>
@@ -3974,7 +4010,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="12" customHeight="1">
+    <row r="58" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44</v>
       </c>
@@ -4030,7 +4066,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="12" customHeight="1">
+    <row r="59" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45</v>
       </c>
@@ -4086,7 +4122,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="12" customHeight="1">
+    <row r="60" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>46</v>
       </c>
@@ -4142,7 +4178,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="12" customHeight="1">
+    <row r="61" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>47</v>
       </c>
@@ -4198,7 +4234,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="12" customHeight="1">
+    <row r="62" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>48</v>
       </c>
@@ -4254,7 +4290,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="12" customHeight="1">
+    <row r="63" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>49</v>
       </c>
@@ -4310,7 +4346,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="12" customHeight="1">
+    <row r="64" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>50</v>
       </c>
@@ -4366,7 +4402,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="12" customHeight="1">
+    <row r="65" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>51</v>
       </c>
@@ -4422,7 +4458,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="12" customHeight="1">
+    <row r="66" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>52</v>
       </c>
@@ -4478,7 +4514,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="12" customHeight="1">
+    <row r="67" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>53</v>
       </c>
@@ -4534,7 +4570,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="12" customHeight="1">
+    <row r="68" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>54</v>
       </c>
@@ -4590,7 +4626,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="12" customHeight="1">
+    <row r="69" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>55</v>
       </c>
@@ -4646,7 +4682,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="12" customHeight="1">
+    <row r="70" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>56</v>
       </c>
@@ -4702,7 +4738,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="12" customHeight="1">
+    <row r="71" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>57</v>
       </c>
@@ -4758,7 +4794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="12" customHeight="1">
+    <row r="72" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>58</v>
       </c>
@@ -4814,7 +4850,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="12" customHeight="1">
+    <row r="73" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>59</v>
       </c>
@@ -4870,7 +4906,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="12" customHeight="1">
+    <row r="74" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>60</v>
       </c>
@@ -4926,7 +4962,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="12" customHeight="1">
+    <row r="75" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>61</v>
       </c>
@@ -4982,7 +5018,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="12" customHeight="1">
+    <row r="76" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>62</v>
       </c>
@@ -5036,7 +5072,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="12" customHeight="1">
+    <row r="77" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>63</v>
       </c>
@@ -5091,45 +5127,31 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:Q1"/>
+  <autoFilter ref="D1:Q1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.75" customWidth="1"/>
+    <col min="2" max="2" width="9.75" customWidth="1"/>
+    <col min="3" max="3" width="27.75" customWidth="1"/>
+    <col min="4" max="18" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" ht="44.15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -5185,7 +5207,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="12" customHeight="1">
+    <row r="2" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5239,7 +5261,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="12" customHeight="1">
+    <row r="3" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5295,7 +5317,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="12" customHeight="1">
+    <row r="4" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5351,7 +5373,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12" customHeight="1">
+    <row r="5" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5407,7 +5429,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="12" customHeight="1">
+    <row r="6" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5463,7 +5485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="12" customHeight="1">
+    <row r="7" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5519,7 +5541,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="12" customHeight="1">
+    <row r="8" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5575,7 +5597,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="12" customHeight="1">
+    <row r="9" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5631,7 +5653,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="12" customHeight="1">
+    <row r="10" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -5687,7 +5709,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="12" customHeight="1">
+    <row r="11" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5743,7 +5765,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="12" customHeight="1">
+    <row r="12" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -5799,7 +5821,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="12" customHeight="1">
+    <row r="13" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -5855,7 +5877,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="12" customHeight="1">
+    <row r="14" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -5911,7 +5933,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="12" customHeight="1">
+    <row r="15" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -5967,7 +5989,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="12" customHeight="1">
+    <row r="16" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -6023,7 +6045,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="12" customHeight="1">
+    <row r="17" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -6079,7 +6101,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="12" customHeight="1">
+    <row r="18" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -6135,7 +6157,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="12" customHeight="1">
+    <row r="19" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -6191,7 +6213,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="12" customHeight="1">
+    <row r="20" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -6247,7 +6269,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="12" customHeight="1">
+    <row r="21" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -6303,7 +6325,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="12" customHeight="1">
+    <row r="22" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -6359,7 +6381,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="12" customHeight="1">
+    <row r="23" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -6415,7 +6437,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="12" customHeight="1">
+    <row r="24" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -6471,7 +6493,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="12" customHeight="1">
+    <row r="25" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -6527,7 +6549,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="12" customHeight="1">
+    <row r="26" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -6583,7 +6605,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="12" customHeight="1">
+    <row r="27" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -6639,7 +6661,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="12" customHeight="1">
+    <row r="28" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -6695,7 +6717,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="12" customHeight="1">
+    <row r="29" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -6751,7 +6773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="12" customHeight="1">
+    <row r="30" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -6807,7 +6829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="12" customHeight="1">
+    <row r="31" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -6863,7 +6885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="12" customHeight="1">
+    <row r="32" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>27</v>
       </c>
@@ -6919,7 +6941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="12" customHeight="1">
+    <row r="33" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>28</v>
       </c>
@@ -6975,7 +6997,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="12" customHeight="1">
+    <row r="34" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>29</v>
       </c>
@@ -7031,7 +7053,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="12" customHeight="1">
+    <row r="35" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>30</v>
       </c>
@@ -7087,7 +7109,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="12" customHeight="1">
+    <row r="36" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>31</v>
       </c>
@@ -7143,7 +7165,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="12" customHeight="1">
+    <row r="37" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>32</v>
       </c>
@@ -7199,7 +7221,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="12" customHeight="1">
+    <row r="38" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>33</v>
       </c>
@@ -7255,7 +7277,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="12" customHeight="1">
+    <row r="39" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>34</v>
       </c>
@@ -7311,7 +7333,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="12" customHeight="1">
+    <row r="40" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>34</v>
       </c>
@@ -7367,7 +7389,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="12" customHeight="1">
+    <row r="41" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>35</v>
       </c>
@@ -7423,7 +7445,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="12" customHeight="1">
+    <row r="42" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>35</v>
       </c>
@@ -7479,7 +7501,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="12" customHeight="1">
+    <row r="43" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>36</v>
       </c>
@@ -7535,7 +7557,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="12" customHeight="1">
+    <row r="44" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>36</v>
       </c>
@@ -7591,7 +7613,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="12" customHeight="1">
+    <row r="45" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>37</v>
       </c>
@@ -7647,7 +7669,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="12" customHeight="1">
+    <row r="46" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>37</v>
       </c>
@@ -7703,7 +7725,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="12" customHeight="1">
+    <row r="47" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>38</v>
       </c>
@@ -7759,7 +7781,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="12" customHeight="1">
+    <row r="48" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>38</v>
       </c>
@@ -7815,7 +7837,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="12" customHeight="1">
+    <row r="49" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>39</v>
       </c>
@@ -7871,7 +7893,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="12" customHeight="1">
+    <row r="50" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>39</v>
       </c>
@@ -7927,7 +7949,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="12" customHeight="1">
+    <row r="51" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>40</v>
       </c>
@@ -7983,7 +8005,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="12" customHeight="1">
+    <row r="52" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>40</v>
       </c>
@@ -8039,7 +8061,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="12" customHeight="1">
+    <row r="53" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>41</v>
       </c>
@@ -8095,7 +8117,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="12" customHeight="1">
+    <row r="54" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>41</v>
       </c>
@@ -8151,7 +8173,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="12" customHeight="1">
+    <row r="55" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>42</v>
       </c>
@@ -8207,7 +8229,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="12" customHeight="1">
+    <row r="56" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>42</v>
       </c>
@@ -8263,7 +8285,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="12" customHeight="1">
+    <row r="57" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43</v>
       </c>
@@ -8319,7 +8341,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="12" customHeight="1">
+    <row r="58" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43</v>
       </c>
@@ -8375,7 +8397,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="12" customHeight="1">
+    <row r="59" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44</v>
       </c>
@@ -8431,7 +8453,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="12" customHeight="1">
+    <row r="60" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44</v>
       </c>
@@ -8487,7 +8509,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="12" customHeight="1">
+    <row r="61" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45</v>
       </c>
@@ -8543,7 +8565,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="12" customHeight="1">
+    <row r="62" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45</v>
       </c>
@@ -8599,7 +8621,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="12" customHeight="1">
+    <row r="63" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>46</v>
       </c>
@@ -8655,7 +8677,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="12" customHeight="1">
+    <row r="64" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>46</v>
       </c>
@@ -8711,7 +8733,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="12" customHeight="1">
+    <row r="65" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>47</v>
       </c>
@@ -8767,7 +8789,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="12" customHeight="1">
+    <row r="66" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>47</v>
       </c>
@@ -8823,7 +8845,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="12" customHeight="1">
+    <row r="67" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>48</v>
       </c>
@@ -8879,7 +8901,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="12" customHeight="1">
+    <row r="68" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>48</v>
       </c>
@@ -8935,7 +8957,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="12" customHeight="1">
+    <row r="69" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>49</v>
       </c>
@@ -8991,7 +9013,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="12" customHeight="1">
+    <row r="70" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>49</v>
       </c>
@@ -9047,7 +9069,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="12" customHeight="1">
+    <row r="71" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>50</v>
       </c>
@@ -9103,7 +9125,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="12" customHeight="1">
+    <row r="72" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>50</v>
       </c>
@@ -9159,7 +9181,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="12" customHeight="1">
+    <row r="73" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>51</v>
       </c>
@@ -9215,7 +9237,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="12" customHeight="1">
+    <row r="74" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>51</v>
       </c>
@@ -9271,7 +9293,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="12" customHeight="1">
+    <row r="75" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>52</v>
       </c>
@@ -9327,7 +9349,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="12" customHeight="1">
+    <row r="76" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>53</v>
       </c>
@@ -9383,7 +9405,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="12" customHeight="1">
+    <row r="77" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>54</v>
       </c>
@@ -9439,7 +9461,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="12" customHeight="1">
+    <row r="78" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>55</v>
       </c>
@@ -9495,7 +9517,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="12" customHeight="1">
+    <row r="79" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>56</v>
       </c>
@@ -9551,7 +9573,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="12" customHeight="1">
+    <row r="80" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>57</v>
       </c>
@@ -9607,7 +9629,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="12" customHeight="1">
+    <row r="81" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>58</v>
       </c>
@@ -9663,7 +9685,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="12" customHeight="1">
+    <row r="82" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>59</v>
       </c>
@@ -9719,7 +9741,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="12" customHeight="1">
+    <row r="83" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>60</v>
       </c>
@@ -9775,7 +9797,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="12" customHeight="1">
+    <row r="84" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>61</v>
       </c>
@@ -9831,7 +9853,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="12" customHeight="1">
+    <row r="85" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>62</v>
       </c>
@@ -9885,7 +9907,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="12" customHeight="1">
+    <row r="86" spans="1:18" ht="12.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>63</v>
       </c>
@@ -9940,7 +9962,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:Q1"/>
+  <autoFilter ref="D1:Q1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>